<commit_message>
got data of Dr.Na
</commit_message>
<xml_diff>
--- a/Samsung_Hospital/SMC_Targets.xlsx
+++ b/Samsung_Hospital/SMC_Targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clmn/Github/labs/Samsung_Hospital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C752B290-180F-CD4D-A3CA-8ED4D47FE3D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CB21F3-A2E5-F049-AEC3-87AA4BBA32A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25500" windowHeight="28340" xr2:uid="{6DFDD1B5-C3B9-B045-81F2-193EDBDAE4AA}"/>
+    <workbookView xWindow="0" yWindow="8640" windowWidth="25580" windowHeight="20160" xr2:uid="{6DFDD1B5-C3B9-B045-81F2-193EDBDAE4AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>patient ID</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -218,7 +218,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3dQWarp 로 인한 차이 확인</t>
+    <t>S42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMN 깔끔하게 구별됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMN과 HF간의 연결이 약함</t>
+  </si>
+  <si>
+    <t>DMN과 HF간의 연결이 약함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3dWarp 로 인한 차이 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -242,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,8 +326,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -300,11 +341,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -314,8 +407,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8F7CE6-4E80-6243-97B6-CB663B4410C2}">
-  <dimension ref="A2:P48"/>
+  <dimension ref="A2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:P29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -648,9 +774,10 @@
     <col min="7" max="11" width="10.7109375" customWidth="1"/>
     <col min="14" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,8 +826,11 @@
       <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -732,12 +862,12 @@
         <v>-18.797000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -769,7 +899,7 @@
         <v>0.41670000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -810,7 +940,7 @@
         <v>0.69754000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -860,7 +990,7 @@
         <v>0.52673999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -910,7 +1040,7 @@
         <v>0.48609999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -930,7 +1060,7 @@
         <v>-13</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -962,7 +1092,7 @@
         <v>0.53949999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1334,24 +1464,24 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
+      <c r="A29" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
@@ -1366,6 +1496,15 @@
       <c r="D30">
         <v>7.1760000000000002</v>
       </c>
+      <c r="E30">
+        <v>-57</v>
+      </c>
+      <c r="F30">
+        <v>-65</v>
+      </c>
+      <c r="G30">
+        <v>33</v>
+      </c>
       <c r="H30">
         <v>-34.545000000000002</v>
       </c>
@@ -1374,6 +1513,15 @@
       </c>
       <c r="J30">
         <v>-27.98</v>
+      </c>
+      <c r="K30">
+        <v>-29</v>
+      </c>
+      <c r="L30">
+        <v>-25</v>
+      </c>
+      <c r="M30">
+        <v>-16</v>
       </c>
       <c r="N30">
         <v>2</v>
@@ -1398,6 +1546,15 @@
       <c r="D31">
         <v>20.209</v>
       </c>
+      <c r="E31">
+        <v>-37</v>
+      </c>
+      <c r="F31">
+        <v>-69</v>
+      </c>
+      <c r="G31">
+        <v>33</v>
+      </c>
       <c r="H31">
         <v>-17.030999999999999</v>
       </c>
@@ -1407,6 +1564,15 @@
       <c r="J31">
         <v>-7.9160000000000004</v>
       </c>
+      <c r="K31">
+        <v>-32</v>
+      </c>
+      <c r="L31">
+        <v>-29</v>
+      </c>
+      <c r="M31">
+        <v>-13</v>
+      </c>
       <c r="N31">
         <v>2</v>
       </c>
@@ -1417,7 +1583,7 @@
         <v>0.64159999999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1430,6 +1596,15 @@
       <c r="D33">
         <v>66.936000000000007</v>
       </c>
+      <c r="E33">
+        <v>-59</v>
+      </c>
+      <c r="F33">
+        <v>-55</v>
+      </c>
+      <c r="G33">
+        <v>42</v>
+      </c>
       <c r="H33">
         <v>-28.837</v>
       </c>
@@ -1439,6 +1614,15 @@
       <c r="J33">
         <v>30.373999999999999</v>
       </c>
+      <c r="K33">
+        <v>-32</v>
+      </c>
+      <c r="L33">
+        <v>-30</v>
+      </c>
+      <c r="M33">
+        <v>-8</v>
+      </c>
       <c r="N33">
         <v>3</v>
       </c>
@@ -1449,7 +1633,7 @@
         <v>0.56920000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1462,6 +1646,15 @@
       <c r="D34">
         <v>20.004999999999999</v>
       </c>
+      <c r="E34">
+        <v>-57</v>
+      </c>
+      <c r="F34">
+        <v>-65</v>
+      </c>
+      <c r="G34">
+        <v>24</v>
+      </c>
       <c r="H34">
         <v>-32.817</v>
       </c>
@@ -1471,6 +1664,15 @@
       <c r="J34">
         <v>-4.8380000000000001</v>
       </c>
+      <c r="K34">
+        <v>-29</v>
+      </c>
+      <c r="L34">
+        <v>-28</v>
+      </c>
+      <c r="M34">
+        <v>-14</v>
+      </c>
       <c r="N34">
         <v>2</v>
       </c>
@@ -1481,7 +1683,7 @@
         <v>0.50009999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1494,6 +1696,15 @@
       <c r="D35">
         <v>44.332999999999998</v>
       </c>
+      <c r="E35">
+        <v>-58</v>
+      </c>
+      <c r="F35">
+        <v>-64</v>
+      </c>
+      <c r="G35">
+        <v>28</v>
+      </c>
       <c r="H35">
         <v>-43.122999999999998</v>
       </c>
@@ -1503,6 +1714,15 @@
       <c r="J35">
         <v>14.798999999999999</v>
       </c>
+      <c r="K35">
+        <v>-29</v>
+      </c>
+      <c r="L35">
+        <v>-30</v>
+      </c>
+      <c r="M35">
+        <v>-11</v>
+      </c>
       <c r="N35">
         <v>2</v>
       </c>
@@ -1513,7 +1733,7 @@
         <v>0.53269999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1526,6 +1746,15 @@
       <c r="D36">
         <v>72.391999999999996</v>
       </c>
+      <c r="E36">
+        <v>-55</v>
+      </c>
+      <c r="F36">
+        <v>-49</v>
+      </c>
+      <c r="G36">
+        <v>30</v>
+      </c>
       <c r="H36">
         <v>-29.113</v>
       </c>
@@ -1535,6 +1764,15 @@
       <c r="J36">
         <v>42.392000000000003</v>
       </c>
+      <c r="K36">
+        <v>-33</v>
+      </c>
+      <c r="L36">
+        <v>-21</v>
+      </c>
+      <c r="M36">
+        <v>-15</v>
+      </c>
       <c r="O36">
         <v>106</v>
       </c>
@@ -1542,7 +1780,7 @@
         <v>0.46589999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1555,6 +1793,15 @@
       <c r="D37">
         <v>55.597999999999999</v>
       </c>
+      <c r="E37">
+        <v>-47</v>
+      </c>
+      <c r="F37">
+        <v>-59</v>
+      </c>
+      <c r="G37">
+        <v>39</v>
+      </c>
       <c r="H37">
         <v>-35.880000000000003</v>
       </c>
@@ -1564,6 +1811,15 @@
       <c r="J37">
         <v>16.690999999999999</v>
       </c>
+      <c r="K37">
+        <v>-35</v>
+      </c>
+      <c r="L37">
+        <v>-29</v>
+      </c>
+      <c r="M37">
+        <v>-13</v>
+      </c>
       <c r="N37">
         <v>2</v>
       </c>
@@ -1574,7 +1830,7 @@
         <v>0.4425</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1587,6 +1843,15 @@
       <c r="D38">
         <v>43.290999999999997</v>
       </c>
+      <c r="E38">
+        <v>-47</v>
+      </c>
+      <c r="F38">
+        <v>-70</v>
+      </c>
+      <c r="G38">
+        <v>29</v>
+      </c>
       <c r="H38">
         <v>-20.283999999999999</v>
       </c>
@@ -1596,6 +1861,15 @@
       <c r="J38">
         <v>9.5410000000000004</v>
       </c>
+      <c r="K38">
+        <v>-34</v>
+      </c>
+      <c r="L38">
+        <v>-27</v>
+      </c>
+      <c r="M38">
+        <v>-16</v>
+      </c>
       <c r="N38">
         <v>2</v>
       </c>
@@ -1606,7 +1880,7 @@
         <v>0.39040000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -1619,6 +1893,15 @@
       <c r="D39">
         <v>-4.6760000000000002</v>
       </c>
+      <c r="E39">
+        <v>-42</v>
+      </c>
+      <c r="F39">
+        <v>-73</v>
+      </c>
+      <c r="G39">
+        <v>34</v>
+      </c>
       <c r="H39">
         <v>-42.85</v>
       </c>
@@ -1628,6 +1911,15 @@
       <c r="J39">
         <v>-29.050999999999998</v>
       </c>
+      <c r="K39">
+        <v>-31</v>
+      </c>
+      <c r="L39">
+        <v>-27</v>
+      </c>
+      <c r="M39">
+        <v>-15</v>
+      </c>
       <c r="N39">
         <v>2</v>
       </c>
@@ -1638,7 +1930,7 @@
         <v>0.59599999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -1651,6 +1943,15 @@
       <c r="D40">
         <v>-11.885999999999999</v>
       </c>
+      <c r="E40">
+        <v>-51</v>
+      </c>
+      <c r="F40">
+        <v>-73</v>
+      </c>
+      <c r="G40">
+        <v>26</v>
+      </c>
       <c r="H40">
         <v>-26.437000000000001</v>
       </c>
@@ -1660,6 +1961,15 @@
       <c r="J40">
         <v>-29.228999999999999</v>
       </c>
+      <c r="K40">
+        <v>-31</v>
+      </c>
+      <c r="L40">
+        <v>-22</v>
+      </c>
+      <c r="M40">
+        <v>-20</v>
+      </c>
       <c r="N40">
         <v>2</v>
       </c>
@@ -1670,7 +1980,23 @@
         <v>0.51329999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="42" spans="1:17">
+      <c r="A42" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q42" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q43" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1683,6 +2009,15 @@
       <c r="D44">
         <v>22.218</v>
       </c>
+      <c r="E44">
+        <v>-45</v>
+      </c>
+      <c r="F44">
+        <v>-75</v>
+      </c>
+      <c r="G44">
+        <v>36</v>
+      </c>
       <c r="H44">
         <v>-35.744</v>
       </c>
@@ -1692,6 +2027,15 @@
       <c r="J44">
         <v>-8.7200000000000006</v>
       </c>
+      <c r="K44">
+        <v>-27</v>
+      </c>
+      <c r="L44">
+        <v>-16</v>
+      </c>
+      <c r="M44">
+        <v>-21</v>
+      </c>
       <c r="N44">
         <v>2</v>
       </c>
@@ -1702,7 +2046,60 @@
         <v>0.52190000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="45" spans="1:17">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>-29.512</v>
+      </c>
+      <c r="C45">
+        <v>-71.819000000000003</v>
+      </c>
+      <c r="D45">
+        <v>17.515999999999998</v>
+      </c>
+      <c r="E45">
+        <v>-32</v>
+      </c>
+      <c r="F45">
+        <v>-82</v>
+      </c>
+      <c r="G45">
+        <v>46</v>
+      </c>
+      <c r="H45">
+        <v>-25.012</v>
+      </c>
+      <c r="I45">
+        <v>-9.9440000000000008</v>
+      </c>
+      <c r="J45">
+        <v>-22.797000000000001</v>
+      </c>
+      <c r="K45">
+        <v>-28</v>
+      </c>
+      <c r="L45">
+        <v>-23</v>
+      </c>
+      <c r="M45">
+        <v>-17</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+      <c r="O45">
+        <v>139</v>
+      </c>
+      <c r="P45">
+        <v>0.43031799999999998</v>
+      </c>
+      <c r="Q45" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1715,6 +2112,15 @@
       <c r="D46">
         <v>51.317999999999998</v>
       </c>
+      <c r="E46">
+        <v>-59</v>
+      </c>
+      <c r="F46">
+        <v>-46</v>
+      </c>
+      <c r="G46">
+        <v>39</v>
+      </c>
       <c r="H46">
         <v>-27.509</v>
       </c>
@@ -1724,6 +2130,15 @@
       <c r="J46">
         <v>11.943</v>
       </c>
+      <c r="K46">
+        <v>-34</v>
+      </c>
+      <c r="L46">
+        <v>-28</v>
+      </c>
+      <c r="M46">
+        <v>-14</v>
+      </c>
       <c r="N46">
         <v>2</v>
       </c>
@@ -1734,7 +2149,60 @@
         <v>0.46050000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="47" spans="1:17">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47">
+        <v>-35.399000000000001</v>
+      </c>
+      <c r="C47">
+        <v>-59.118000000000002</v>
+      </c>
+      <c r="D47">
+        <v>49.713000000000001</v>
+      </c>
+      <c r="E47">
+        <v>-33</v>
+      </c>
+      <c r="F47">
+        <v>-86</v>
+      </c>
+      <c r="G47">
+        <v>35</v>
+      </c>
+      <c r="H47">
+        <v>-31.899000000000001</v>
+      </c>
+      <c r="I47">
+        <v>-10.368</v>
+      </c>
+      <c r="J47">
+        <v>11.275</v>
+      </c>
+      <c r="K47">
+        <v>-31</v>
+      </c>
+      <c r="L47">
+        <v>-30</v>
+      </c>
+      <c r="M47">
+        <v>-11</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+      <c r="O47">
+        <v>112</v>
+      </c>
+      <c r="P47">
+        <v>0.46599600000000002</v>
+      </c>
+      <c r="Q47" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1747,6 +2215,15 @@
       <c r="D48">
         <v>28.373999999999999</v>
       </c>
+      <c r="E48">
+        <v>-54</v>
+      </c>
+      <c r="F48">
+        <v>-56</v>
+      </c>
+      <c r="G48">
+        <v>20</v>
+      </c>
       <c r="H48">
         <v>-37.064999999999998</v>
       </c>
@@ -1756,6 +2233,15 @@
       <c r="J48">
         <v>2.1240000000000001</v>
       </c>
+      <c r="K48">
+        <v>-33</v>
+      </c>
+      <c r="L48">
+        <v>-25</v>
+      </c>
+      <c r="M48">
+        <v>-15</v>
+      </c>
       <c r="N48">
         <v>2</v>
       </c>
@@ -1765,6 +2251,44 @@
       <c r="P48">
         <v>0.43059999999999998</v>
       </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="15">
+        <f>AVERAGE(E$3:E$28,E$30:E$48)</f>
+        <v>-49.761904761904759</v>
+      </c>
+      <c r="F53" s="12">
+        <f t="shared" ref="F53:G53" si="0">AVERAGE(F$3:F$28,F$30:F$48)</f>
+        <v>-66.714285714285708</v>
+      </c>
+      <c r="G53" s="16">
+        <f t="shared" si="0"/>
+        <v>32.952380952380949</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="17">
+        <f>AVERAGE(K$3:K$28,K$30:K$48)</f>
+        <v>-30.863636363636363</v>
+      </c>
+      <c r="L53" s="13">
+        <f t="shared" ref="L53:M53" si="1">AVERAGE(L$3:L$28,L$30:L$48)</f>
+        <v>-25.818181818181817</v>
+      </c>
+      <c r="M53" s="18">
+        <f t="shared" si="1"/>
+        <v>-15.136363636363637</v>
+      </c>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ready to summit S39, S40
</commit_message>
<xml_diff>
--- a/Samsung_Hospital/SMC_Targets.xlsx
+++ b/Samsung_Hospital/SMC_Targets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clmn/Github/labs/Samsung_Hospital/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEA30F2-2FDA-A545-A188-CD646A3FBEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9234FCC6-D2A2-7E45-8A18-51C977E19CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8640" windowWidth="25580" windowHeight="20160" xr2:uid="{6DFDD1B5-C3B9-B045-81F2-193EDBDAE4AA}"/>
+    <workbookView xWindow="0" yWindow="8540" windowWidth="25500" windowHeight="20260" xr2:uid="{6DFDD1B5-C3B9-B045-81F2-193EDBDAE4AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>patient ID</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -242,13 +242,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DMN과 HF간의 연결이 약함</t>
-  </si>
-  <si>
-    <t>DMN과 HF간의 연결이 약함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3dWarp 로 인한 차이 확인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -275,6 +268,10 @@
   </si>
   <si>
     <t>총원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeuroSynth의 AG 좌표를 사용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -360,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -375,19 +372,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -424,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -443,34 +427,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -792,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8F7CE6-4E80-6243-97B6-CB663B4410C2}">
   <dimension ref="A2:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -802,7 +776,7 @@
     <col min="7" max="11" width="10.7109375" customWidth="1"/>
     <col min="14" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.5703125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17">
@@ -1492,24 +1466,24 @@
       </c>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="18"/>
+      <c r="A29" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" t="s">
@@ -2010,7 +1984,7 @@
     </row>
     <row r="41" spans="1:17">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41">
         <v>-55.204999999999998</v>
@@ -2062,16 +2036,88 @@
       <c r="A42" t="s">
         <v>52</v>
       </c>
+      <c r="B42">
+        <v>-49.314</v>
+      </c>
+      <c r="C42">
+        <v>-60.945999999999998</v>
+      </c>
+      <c r="D42">
+        <v>-9.0150000000000006</v>
+      </c>
+      <c r="E42" s="14">
+        <v>-48</v>
+      </c>
+      <c r="F42" s="14">
+        <v>-70</v>
+      </c>
+      <c r="G42" s="14">
+        <v>38</v>
+      </c>
+      <c r="H42">
+        <v>-29.814</v>
+      </c>
+      <c r="I42">
+        <v>-8.9139999999999997</v>
+      </c>
+      <c r="J42">
+        <v>-35.265000000000001</v>
+      </c>
+      <c r="K42" s="14">
+        <v>-28</v>
+      </c>
+      <c r="L42" s="14">
+        <v>-24</v>
+      </c>
+      <c r="M42" s="14">
+        <v>-16</v>
+      </c>
       <c r="Q42" s="8" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:17">
       <c r="A43" t="s">
         <v>53</v>
       </c>
+      <c r="B43">
+        <v>-40.191000000000003</v>
+      </c>
+      <c r="C43">
+        <v>-70.503</v>
+      </c>
+      <c r="D43">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="E43" s="14">
+        <v>-48</v>
+      </c>
+      <c r="F43" s="14">
+        <v>-70</v>
+      </c>
+      <c r="G43" s="14">
+        <v>38</v>
+      </c>
+      <c r="H43" s="17">
+        <v>-20.690999999999999</v>
+      </c>
+      <c r="I43" s="17">
+        <v>13.784000000000001</v>
+      </c>
+      <c r="J43" s="17">
+        <v>-27.103000000000002</v>
+      </c>
+      <c r="K43" s="14">
+        <v>-28</v>
+      </c>
+      <c r="L43" s="14">
+        <v>-24</v>
+      </c>
+      <c r="M43" s="14">
+        <v>-16</v>
+      </c>
       <c r="Q43" s="8" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -2332,7 +2378,7 @@
     </row>
     <row r="49" spans="1:16">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B49">
         <v>-40.811</v>
@@ -2382,7 +2428,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B50">
         <v>-55.335000000000001</v>
@@ -2432,7 +2478,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B51">
         <v>-57.146000000000001</v>
@@ -2481,49 +2527,49 @@
       </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="19" t="s">
-        <v>61</v>
+      <c r="A52" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" s="14">
-        <f>AVERAGE(E$3:E$28,E$30:E$51)</f>
+        <v>55</v>
+      </c>
+      <c r="E53" s="16">
+        <f>AVERAGE(E$3:E$28,E$30:E$41,E$44:E$51)</f>
         <v>-49.92</v>
       </c>
-      <c r="F53" s="11">
-        <f>AVERAGE(F$3:F$28,F$30:F$51)</f>
+      <c r="F53" s="16">
+        <f>AVERAGE(F$3:F$28,F$30:F$41,F$44:F$51)</f>
         <v>-66.599999999999994</v>
       </c>
-      <c r="G53" s="15">
-        <f>AVERAGE(G$3:G$28,G$30:G$51)</f>
+      <c r="G53" s="16">
+        <f t="shared" ref="F53:G53" si="0">AVERAGE(G$3:G$28,G$30:G$41,G$44:G$51)</f>
         <v>32.72</v>
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
-      <c r="K53" s="16">
-        <f>AVERAGE(K$3:K$28,K$30:K$51)</f>
+      <c r="K53" s="15">
+        <f>AVERAGE(K$3:K$28,K$30:K$41,K$44:K$51)</f>
         <v>-30.653846153846153</v>
       </c>
-      <c r="L53" s="12">
-        <f>AVERAGE(L$3:L$28,L$30:L$51)</f>
+      <c r="L53" s="15">
+        <f>AVERAGE(L$3:L$28,L$30:L$41,L$44:L$51)</f>
         <v>-26.346153846153847</v>
       </c>
-      <c r="M53" s="17">
-        <f>AVERAGE(M$3:M$28,M$30:M$51)</f>
+      <c r="M53" s="15">
+        <f>AVERAGE(M$3:M$28,M$30:M$41,M$44:M$51)</f>
         <v>-14.961538461538462</v>
       </c>
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
-      <c r="P53" s="13"/>
+      <c r="P53" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>